<commit_message>
updates to utils and no more separate calibrant run
</commit_message>
<xml_diff>
--- a/agilent_methods/experimentTemplate_short.xlsx
+++ b/agilent_methods/experimentTemplate_short.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t xml:space="preserve">Well</t>
   </si>
@@ -56,22 +56,43 @@
     <t xml:space="preserve">B1</t>
   </si>
   <si>
+    <t xml:space="preserve">Tune Mix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-02_dodd_4bit_POS.m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P384</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2</t>
+  </si>
+  <si>
     <t xml:space="preserve">IPA Blank</t>
   </si>
   <si>
-    <t xml:space="preserve">Positive</t>
-  </si>
-  <si>
     <t xml:space="preserve">BLANK</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-03-02_dodd_4bit_POS.m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P384</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
+    <t xml:space="preserve">B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1</t>
   </si>
   <si>
     <t xml:space="preserve">Negative</t>
@@ -80,7 +101,10 @@
     <t xml:space="preserve">2023-03-02_dodd_4bit_NEG.m</t>
   </si>
   <si>
-    <t xml:space="preserve">e</t>
+    <t xml:space="preserve">C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3</t>
   </si>
   <si>
     <t xml:space="preserve">Parameter</t>
@@ -313,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -360,7 +384,7 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -387,13 +411,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -402,10 +426,10 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -414,9 +438,120 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G6" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -448,15 +583,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1.5</v>
@@ -464,7 +599,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>0</v>
@@ -472,7 +607,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0</v>
@@ -480,7 +615,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
@@ -488,7 +623,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -497,7 +632,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -506,7 +641,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -515,7 +650,7 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -524,7 +659,7 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1.25</v>
@@ -532,7 +667,7 @@
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>0.01</v>
@@ -540,7 +675,7 @@
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>0.01</v>
@@ -548,7 +683,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>-1</v>
@@ -556,7 +691,7 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>-1</v>
@@ -564,7 +699,7 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>-1</v>
@@ -572,7 +707,7 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>-1</v>
@@ -580,7 +715,7 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>-1</v>
@@ -588,7 +723,7 @@
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>-1</v>
@@ -596,7 +731,7 @@
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>-1</v>
@@ -604,7 +739,7 @@
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>50</v>
@@ -618,7 +753,7 @@
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>100</v>
@@ -632,7 +767,7 @@
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>100</v>
@@ -646,7 +781,7 @@
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -655,7 +790,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -664,7 +799,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -673,7 +808,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="b">
         <f aca="false">FALSE()</f>
@@ -682,7 +817,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>0</v>
@@ -690,15 +825,15 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>10000</v>
@@ -706,27 +841,27 @@
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>600</v>

</xml_diff>